<commit_message>
Add updated budget, worksheet, and narrative from T. Libert.
</commit_message>
<xml_diff>
--- a/assets/Software Engr_osu_internal_budget_worksheet.xlsx
+++ b/assets/Software Engr_osu_internal_budget_worksheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="465" windowWidth="23115" windowHeight="15435" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="463" windowWidth="23117" windowHeight="15437" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Recurring" sheetId="1" r:id="rId1"/>
@@ -1278,17 +1278,17 @@
   </sheetPr>
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="5" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.84375" customWidth="1"/>
+    <col min="2" max="5" width="14.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="19.75" x14ac:dyDescent="0.45">
       <c r="A1" s="89" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="D1" s="89"/>
       <c r="E1" s="89"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
         <v>14</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="D2" s="88"/>
       <c r="E2" s="88"/>
     </row>
-    <row r="3" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="87" t="s">
         <v>24</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="D3" s="87"/>
       <c r="E3" s="87"/>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
         <v>26</v>
       </c>
@@ -1332,14 +1332,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19"/>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
     </row>
-    <row r="7" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
@@ -1356,17 +1356,17 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="20"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="91" t="s">
         <v>25</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="E10" s="93"/>
       <c r="F10" s="84"/>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="8"/>
       <c r="B11" s="21" t="s">
         <v>30</v>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="F11" s="84"/>
     </row>
-    <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="22" t="s">
         <v>0</v>
       </c>
@@ -1401,13 +1401,13 @@
       <c r="E12" s="9"/>
       <c r="F12" s="84"/>
     </row>
-    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="67"/>
       <c r="C13" s="67">
-        <f t="shared" ref="C13:E13" si="0">ROUND(B13*1.02,0)</f>
+        <f t="shared" ref="C13:D13" si="0">ROUND(B13*1.02,0)</f>
         <v>0</v>
       </c>
       <c r="D13" s="67">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="F13" s="84"/>
     </row>
-    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="23" t="s">
         <v>2</v>
       </c>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="F14" s="84"/>
     </row>
-    <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="24" t="s">
         <v>22</v>
       </c>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="F15" s="84"/>
     </row>
-    <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="23" t="s">
         <v>3</v>
       </c>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="F16" s="84"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="23" t="s">
         <v>4</v>
       </c>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="F17" s="84"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="23" t="s">
         <v>23</v>
       </c>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="F18" s="84"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="23" t="s">
         <v>5</v>
       </c>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="F19" s="84"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="25" t="s">
         <v>15</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="F20" s="84"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="84"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="73" t="s">
         <v>38</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="F22" s="84"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="73" t="s">
         <v>39</v>
       </c>
@@ -1597,12 +1597,12 @@
       </c>
       <c r="F23" s="84"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="67">
-        <v>3787.5</v>
+        <v>4472.5</v>
       </c>
       <c r="C24" s="67">
         <v>4500</v>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="F24" s="84"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="23" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +1625,7 @@
       <c r="E25" s="68"/>
       <c r="F25" s="84"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="23" t="s">
         <v>9</v>
       </c>
@@ -1635,13 +1635,13 @@
       <c r="E26" s="68"/>
       <c r="F26" s="84"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="3">
         <f>SUM(B22:B26)</f>
-        <v>3787.5</v>
+        <v>4472.5</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" ref="C27:E27" si="1">SUM(C22:C26)</f>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="F27" s="84"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="26"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1665,13 +1665,13 @@
       <c r="E28" s="12"/>
       <c r="F28" s="84"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A29" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="15">
         <f>B20+B27</f>
-        <v>132831.03190515365</v>
+        <v>133516.03190515365</v>
       </c>
       <c r="C29" s="15">
         <f>C20+C27</f>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="F29" s="84"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="28"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -1695,7 +1695,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="84"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="22" t="s">
         <v>10</v>
       </c>
@@ -1705,19 +1705,19 @@
       <c r="E31" s="11"/>
       <c r="F31" s="84"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="23" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="67">
-        <v>13995</v>
+        <v>14680</v>
       </c>
       <c r="C32" s="67"/>
       <c r="D32" s="67"/>
       <c r="E32" s="68"/>
       <c r="F32" s="84"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="23" t="s">
         <v>11</v>
       </c>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="F33" s="84"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="23" t="s">
         <v>12</v>
       </c>
@@ -1745,7 +1745,7 @@
       <c r="E34" s="68"/>
       <c r="F34" s="84"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="23" t="s">
         <v>16</v>
       </c>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="F35" s="84"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="64" t="s">
         <v>40</v>
       </c>
@@ -1773,7 +1773,7 @@
       <c r="E36" s="68"/>
       <c r="F36" s="84"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="64" t="s">
         <v>41</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="E37" s="68"/>
       <c r="F37" s="84"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="65"/>
       <c r="B38" s="69"/>
       <c r="C38" s="69"/>
@@ -1791,13 +1791,13 @@
       <c r="E38" s="70"/>
       <c r="F38" s="84"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="17">
         <f t="shared" ref="B39:D39" si="3">SUM(B32:B38)</f>
-        <v>132830.60507034574</v>
+        <v>133515.60507034574</v>
       </c>
       <c r="C39" s="17">
         <f t="shared" si="3"/>
@@ -1813,13 +1813,13 @@
       </c>
       <c r="F39" s="84"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
@@ -1828,19 +1828,19 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="86" t="s">
         <v>42</v>
       </c>
@@ -1861,92 +1861,92 @@
         <v>-109765.05222206679</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="5">
@@ -1981,16 +1981,16 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="5" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.84375" customWidth="1"/>
+    <col min="2" max="5" width="14.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="19.75" x14ac:dyDescent="0.45">
       <c r="A1" s="89" t="s">
         <v>13</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="D1" s="89"/>
       <c r="E1" s="89"/>
     </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
         <v>14</v>
       </c>
@@ -2008,7 +2008,7 @@
       <c r="D2" s="88"/>
       <c r="E2" s="88"/>
     </row>
-    <row r="3" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="87" t="s">
         <v>24</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="D3" s="87"/>
       <c r="E3" s="87"/>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
         <v>26</v>
       </c>
@@ -2035,14 +2035,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19"/>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
     </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
@@ -2061,17 +2061,17 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="20"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="91" t="s">
         <v>34</v>
       </c>
@@ -2080,7 +2080,7 @@
       <c r="E10" s="93"/>
       <c r="F10" s="84"/>
     </row>
-    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="8"/>
       <c r="B11" s="21" t="s">
         <v>30</v>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="F11" s="84"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="22" t="s">
         <v>0</v>
       </c>
@@ -2106,7 +2106,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="84"/>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="23" t="s">
         <v>1</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="F13" s="84"/>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="23" t="s">
         <v>2</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="E14" s="68"/>
       <c r="F14" s="84"/>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="24" t="s">
         <v>22</v>
       </c>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="F15" s="84"/>
     </row>
-    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="23" t="s">
         <v>3</v>
       </c>
@@ -2166,7 +2166,7 @@
       <c r="E16" s="68"/>
       <c r="F16" s="84"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="23" t="s">
         <v>4</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="E17" s="68"/>
       <c r="F17" s="84"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="23" t="s">
         <v>23</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="E18" s="68"/>
       <c r="F18" s="84"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="23" t="s">
         <v>5</v>
       </c>
@@ -2196,7 +2196,7 @@
       <c r="E19" s="68"/>
       <c r="F19" s="84"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="25" t="s">
         <v>15</v>
       </c>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="F20" s="84"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
         <v>6</v>
       </c>
@@ -2228,7 +2228,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="84"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="75" t="s">
         <v>38</v>
       </c>
@@ -2238,7 +2238,7 @@
       <c r="E22" s="77"/>
       <c r="F22" s="84"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="75" t="s">
         <v>39</v>
       </c>
@@ -2248,23 +2248,21 @@
       <c r="E23" s="77"/>
       <c r="F23" s="84"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="67">
-        <v>4225</v>
-      </c>
+      <c r="B24" s="67"/>
       <c r="C24" s="67"/>
       <c r="D24" s="67">
-        <v>2000</v>
+        <v>6225</v>
       </c>
       <c r="E24" s="68">
         <v>27000</v>
       </c>
       <c r="F24" s="84"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="23" t="s">
         <v>8</v>
       </c>
@@ -2274,7 +2272,7 @@
       <c r="E25" s="68"/>
       <c r="F25" s="84"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="23" t="s">
         <v>9</v>
       </c>
@@ -2284,13 +2282,13 @@
       <c r="E26" s="68"/>
       <c r="F26" s="84"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="3">
         <f>SUM(B22:B26)</f>
-        <v>4225</v>
+        <v>0</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" ref="C27:E27" si="0">SUM(C22:C26)</f>
@@ -2298,7 +2296,7 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>6225</v>
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
@@ -2306,7 +2304,7 @@
       </c>
       <c r="F27" s="84"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="26"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2314,13 +2312,13 @@
       <c r="E28" s="12"/>
       <c r="F28" s="84"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A29" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="15">
         <f>B20+B27</f>
-        <v>4225</v>
+        <v>0</v>
       </c>
       <c r="C29" s="15">
         <f>C20+C27</f>
@@ -2328,7 +2326,7 @@
       </c>
       <c r="D29" s="15">
         <f>D20+D27</f>
-        <v>2000</v>
+        <v>6225</v>
       </c>
       <c r="E29" s="16">
         <f>E20+E27</f>
@@ -2336,7 +2334,7 @@
       </c>
       <c r="F29" s="84"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="28"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -2344,7 +2342,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="84"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="22" t="s">
         <v>10</v>
       </c>
@@ -2354,19 +2352,17 @@
       <c r="E31" s="11"/>
       <c r="F31" s="84"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="67">
-        <v>4225</v>
-      </c>
+      <c r="B32" s="67"/>
       <c r="C32" s="67"/>
       <c r="D32" s="67"/>
       <c r="E32" s="68"/>
       <c r="F32" s="84"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="23" t="s">
         <v>11</v>
       </c>
@@ -2376,7 +2372,7 @@
       <c r="E33" s="68"/>
       <c r="F33" s="84"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="23" t="s">
         <v>12</v>
       </c>
@@ -2386,7 +2382,7 @@
       <c r="E34" s="68"/>
       <c r="F34" s="84"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="23" t="s">
         <v>16</v>
       </c>
@@ -2396,7 +2392,7 @@
       <c r="E35" s="68"/>
       <c r="F35" s="84"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="64"/>
       <c r="B36" s="67"/>
       <c r="C36" s="67"/>
@@ -2404,7 +2400,7 @@
       <c r="E36" s="68"/>
       <c r="F36" s="84"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="64"/>
       <c r="B37" s="67"/>
       <c r="C37" s="67"/>
@@ -2412,7 +2408,7 @@
       <c r="E37" s="68"/>
       <c r="F37" s="84"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="65"/>
       <c r="B38" s="69"/>
       <c r="C38" s="69"/>
@@ -2420,13 +2416,13 @@
       <c r="E38" s="70"/>
       <c r="F38" s="84"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="17">
         <f t="shared" ref="B39:D39" si="1">SUM(B32:B38)</f>
-        <v>4225</v>
+        <v>0</v>
       </c>
       <c r="C39" s="17">
         <f t="shared" si="1"/>
@@ -2442,13 +2438,13 @@
       </c>
       <c r="F39" s="84"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
@@ -2457,13 +2453,13 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2477,105 +2473,105 @@
       </c>
       <c r="D43" s="6">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>6225</v>
       </c>
       <c r="E43" s="6">
         <f t="shared" si="2"/>
         <v>27000</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <sheetProtection password="CC94" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="5">
@@ -2607,17 +2603,17 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="34" customWidth="1"/>
-    <col min="2" max="5" width="14.85546875" style="34" customWidth="1"/>
-    <col min="6" max="16384" width="7.42578125" style="34"/>
+    <col min="1" max="1" width="33.84375" style="34" customWidth="1"/>
+    <col min="2" max="5" width="14.84375" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="7.3828125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="19.75" x14ac:dyDescent="0.45">
       <c r="A1" s="95" t="s">
         <v>13</v>
       </c>
@@ -2626,7 +2622,7 @@
       <c r="D1" s="95"/>
       <c r="E1" s="95"/>
     </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="96" t="s">
         <v>14</v>
       </c>
@@ -2635,7 +2631,7 @@
       <c r="D2" s="96"/>
       <c r="E2" s="96"/>
     </row>
-    <row r="3" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="97" t="s">
         <v>24</v>
       </c>
@@ -2644,7 +2640,7 @@
       <c r="D3" s="97"/>
       <c r="E3" s="97"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="L4" s="66" t="s">
         <v>36</v>
       </c>
@@ -2652,7 +2648,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="35" t="s">
         <v>26</v>
       </c>
@@ -2664,14 +2660,14 @@
       <c r="D5" s="98"/>
       <c r="E5" s="98"/>
     </row>
-    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
       <c r="E6" s="36"/>
     </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="35" t="s">
         <v>27</v>
       </c>
@@ -2690,17 +2686,17 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="35"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
       <c r="E8" s="36"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="39"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="99" t="s">
         <v>35</v>
       </c>
@@ -2708,7 +2704,7 @@
       <c r="D10" s="100"/>
       <c r="E10" s="101"/>
     </row>
-    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="40"/>
       <c r="B11" s="41" t="s">
         <v>30</v>
@@ -2723,7 +2719,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="43" t="s">
         <v>0</v>
       </c>
@@ -2732,7 +2728,7 @@
       <c r="D12" s="44"/>
       <c r="E12" s="45"/>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="46" t="s">
         <v>1</v>
       </c>
@@ -2753,7 +2749,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="46" t="s">
         <v>2</v>
       </c>
@@ -2774,7 +2770,7 @@
         <v>181319.14369631128</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="49" t="s">
         <v>22</v>
       </c>
@@ -2795,7 +2791,7 @@
         <v>281319.14369631128</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="46" t="s">
         <v>3</v>
       </c>
@@ -2816,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="46" t="s">
         <v>4</v>
       </c>
@@ -2837,7 +2833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="46" t="s">
         <v>23</v>
       </c>
@@ -2858,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="46" t="s">
         <v>5</v>
       </c>
@@ -2879,7 +2875,7 @@
         <v>183183.73402534626</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="50" t="s">
         <v>15</v>
       </c>
@@ -2900,7 +2896,7 @@
         <v>464502.87772165751</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="43" t="s">
         <v>6</v>
       </c>
@@ -2909,7 +2905,7 @@
       <c r="D21" s="51"/>
       <c r="E21" s="52"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="74" t="s">
         <v>38</v>
       </c>
@@ -2930,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="74" t="s">
         <v>39</v>
       </c>
@@ -2951,13 +2947,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="46" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="47">
         <f>SUM(Recurring!B24,'One-time'!B24)</f>
-        <v>8012.5</v>
+        <v>4472.5</v>
       </c>
       <c r="C24" s="47">
         <f>SUM(Recurring!C24,'One-time'!C24)</f>
@@ -2965,14 +2961,14 @@
       </c>
       <c r="D24" s="47">
         <f>SUM(Recurring!D24,'One-time'!D24)</f>
-        <v>10270</v>
+        <v>14495</v>
       </c>
       <c r="E24" s="48">
         <f>SUM(Recurring!E24,'One-time'!E24)</f>
         <v>39295</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="46" t="s">
         <v>8</v>
       </c>
@@ -2993,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="46" t="s">
         <v>9</v>
       </c>
@@ -3014,13 +3010,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="50" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="47">
         <f>SUM(B22:B26)</f>
-        <v>8012.5</v>
+        <v>4472.5</v>
       </c>
       <c r="C27" s="47">
         <f t="shared" ref="C27:D27" si="0">SUM(C22:C26)</f>
@@ -3028,27 +3024,27 @@
       </c>
       <c r="D27" s="47">
         <f t="shared" si="0"/>
-        <v>10270</v>
+        <v>14495</v>
       </c>
       <c r="E27" s="48">
         <f>SUM(E22:E26)</f>
         <v>39295</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="53"/>
       <c r="B28" s="54"/>
       <c r="C28" s="54"/>
       <c r="D28" s="54"/>
       <c r="E28" s="55"/>
     </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A29" s="56" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="57">
         <f>B20+B27</f>
-        <v>137056.03190515365</v>
+        <v>133516.03190515365</v>
       </c>
       <c r="C29" s="57">
         <f>C20+C27</f>
@@ -3056,21 +3052,21 @@
       </c>
       <c r="D29" s="57">
         <f>D20+D27</f>
-        <v>317517.52040479775</v>
+        <v>321742.52040479775</v>
       </c>
       <c r="E29" s="58">
         <f>E20+E27</f>
         <v>503797.87772165751</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="59"/>
       <c r="B30" s="60"/>
       <c r="C30" s="60"/>
       <c r="D30" s="60"/>
       <c r="E30" s="61"/>
     </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="43" t="s">
         <v>10</v>
       </c>
@@ -3079,13 +3075,13 @@
       <c r="D31" s="51"/>
       <c r="E31" s="52"/>
     </row>
-    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="46" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="47">
         <f>SUM(Recurring!B32,'One-time'!B32)</f>
-        <v>18220</v>
+        <v>14680</v>
       </c>
       <c r="C32" s="47">
         <f>SUM(Recurring!C32,'One-time'!C32)</f>
@@ -3100,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="46" t="s">
         <v>11</v>
       </c>
@@ -3121,7 +3117,7 @@
         <v>489714.51077505015</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="46" t="s">
         <v>12</v>
       </c>
@@ -3142,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="46" t="s">
         <v>16</v>
       </c>
@@ -3163,7 +3159,7 @@
         <v>96848.419168674183</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="64" t="s">
         <v>40</v>
       </c>
@@ -3184,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="64" t="s">
         <v>41</v>
       </c>
@@ -3205,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="78"/>
       <c r="B38" s="79">
         <f>SUM(Recurring!B38,'One-time'!B38)</f>
@@ -3224,16 +3220,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="81" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="82">
         <f>SUM(B32:B38)</f>
-        <v>137055.60507034574</v>
+        <v>133515.60507034574</v>
       </c>
       <c r="C39" s="82">
-        <f t="shared" ref="B39:D39" si="1">SUM(C32:C38)</f>
+        <f t="shared" ref="C39:D39" si="1">SUM(C32:C38)</f>
         <v>253426.7106569102</v>
       </c>
       <c r="D39" s="82">
@@ -3245,13 +3241,13 @@
         <v>586562.9299437243</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="62"/>
       <c r="C40" s="62"/>
       <c r="D40" s="62"/>
       <c r="E40" s="62"/>
     </row>
-    <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="63" t="s">
         <v>19</v>
       </c>
@@ -3260,110 +3256,110 @@
       <c r="D41" s="62"/>
       <c r="E41" s="62"/>
     </row>
-    <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="62"/>
       <c r="C42" s="62"/>
       <c r="D42" s="62"/>
       <c r="E42" s="62"/>
     </row>
-    <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" s="62"/>
       <c r="C43" s="62"/>
       <c r="D43" s="62"/>
       <c r="E43" s="62"/>
     </row>
-    <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B44" s="62"/>
       <c r="C44" s="62"/>
       <c r="D44" s="62"/>
       <c r="E44" s="62"/>
     </row>
-    <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="62"/>
       <c r="C45" s="62"/>
       <c r="D45" s="62"/>
       <c r="E45" s="62"/>
     </row>
-    <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" s="62"/>
       <c r="C46" s="62"/>
       <c r="D46" s="62"/>
       <c r="E46" s="62"/>
     </row>
-    <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B47" s="62"/>
       <c r="C47" s="62"/>
       <c r="D47" s="62"/>
       <c r="E47" s="62"/>
     </row>
-    <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B48" s="62"/>
       <c r="C48" s="62"/>
       <c r="D48" s="62"/>
       <c r="E48" s="62"/>
     </row>
-    <row r="49" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="62"/>
       <c r="C49" s="62"/>
       <c r="D49" s="62"/>
       <c r="E49" s="62"/>
     </row>
-    <row r="50" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="62"/>
       <c r="C50" s="62"/>
       <c r="D50" s="62"/>
       <c r="E50" s="62"/>
     </row>
-    <row r="51" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="62"/>
       <c r="C51" s="62"/>
       <c r="D51" s="62"/>
       <c r="E51" s="62"/>
     </row>
-    <row r="52" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="62"/>
       <c r="C52" s="62"/>
       <c r="D52" s="62"/>
       <c r="E52" s="62"/>
     </row>
-    <row r="53" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" s="62"/>
       <c r="C53" s="62"/>
       <c r="D53" s="62"/>
       <c r="E53" s="62"/>
     </row>
-    <row r="54" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="62"/>
       <c r="C54" s="62"/>
       <c r="D54" s="62"/>
       <c r="E54" s="62"/>
     </row>
-    <row r="55" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="62"/>
       <c r="C55" s="62"/>
       <c r="D55" s="62"/>
       <c r="E55" s="62"/>
     </row>
-    <row r="56" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B56" s="62"/>
       <c r="C56" s="62"/>
       <c r="D56" s="62"/>
       <c r="E56" s="62"/>
     </row>
-    <row r="57" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="62"/>
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
       <c r="E57" s="62"/>
     </row>
-    <row r="58" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="16.5" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="5">

</xml_diff>